<commit_message>
Update data files - Bot run at 2026-02-12 15:39:51 UTC
</commit_message>
<xml_diff>
--- a/dm_promotion_service/data/users_engagement.xlsx
+++ b/dm_promotion_service/data/users_engagement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -703,6 +703,39 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6698418542</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sourabratabose</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>unreachable</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Added during extraction</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 20:44:22 UTC
</commit_message>
<xml_diff>
--- a/dm_promotion_service/data/users_engagement.xlsx
+++ b/dm_promotion_service/data/users_engagement.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,64 +434,102 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>user_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>username</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>level</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>last_message_date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>last_response</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>response_status</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>level_3_ai_response</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>subscription_checked</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>level_4_reminder_sent</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>decision</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>first_added_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>8192984600</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>user_8192984600</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-02-13T20:43:55.614256+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Added during extraction</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 05:00:10 UTC
</commit_message>
<xml_diff>
--- a/dm_promotion_service/data/users_engagement.xlsx
+++ b/dm_promotion_service/data/users_engagement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,6 +533,44 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1594575966</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>user_1594575966</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2026-02-14T04:59:35.710181+00:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Added during extraction</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2026-02-14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>